<commit_message>
sems removed, electricity price name revised
</commit_message>
<xml_diff>
--- a/data/input/Scenario_Component_EnergyPrice.xlsx
+++ b/data/input/Scenario_Component_EnergyPrice.xlsx
@@ -30,13 +30,13 @@
     <t>cent/Wh</t>
   </si>
   <si>
-    <t>id_electricity_consumption</t>
-  </si>
-  <si>
     <t>id_electricity_feed_in</t>
   </si>
   <si>
     <t>id_gases</t>
+  </si>
+  <si>
+    <t>id_electricity</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID_EnergyPrice"/>
-    <tableColumn id="2" name="id_electricity_consumption"/>
+    <tableColumn id="2" name="id_electricity"/>
     <tableColumn id="3" name="id_electricity_feed_in"/>
     <tableColumn id="4" name="id_gases"/>
     <tableColumn id="5" name="price_unit"/>
@@ -392,7 +392,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,13 +409,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>

</xml_diff>